<commit_message>
push to new folder
</commit_message>
<xml_diff>
--- a/Resources DO NOT EDIT/rachel_data/island_pca.xlsx
+++ b/Resources DO NOT EDIT/rachel_data/island_pca.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/R Projects/Happy_Hour_2/Bill/data/rachel_pca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF282FA9-2B8B-424D-A754-89782594E8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE16E07-0E06-064C-B8D0-AC40F9CDD6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="3140" windowWidth="28040" windowHeight="17440" xr2:uid="{F818C2FF-556E-AA40-81CE-D80026F9CBC8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="227">
   <si>
     <t>trapping_code</t>
   </si>
@@ -1071,10 +1071,13 @@
   <dimension ref="A1:L205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K178" sqref="K178:K205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7830,11 +7833,11 @@
       <c r="I178">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J178" t="s">
-        <v>22</v>
-      </c>
-      <c r="K178" t="s">
-        <v>22</v>
+      <c r="J178">
+        <v>31285000000</v>
+      </c>
+      <c r="K178">
+        <v>0</v>
       </c>
       <c r="L178">
         <v>31</v>
@@ -7868,11 +7871,11 @@
       <c r="I179">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J179" t="s">
-        <v>22</v>
-      </c>
-      <c r="K179" t="s">
-        <v>22</v>
+      <c r="J179">
+        <v>31285000000</v>
+      </c>
+      <c r="K179">
+        <v>0</v>
       </c>
       <c r="L179">
         <v>31</v>
@@ -7906,11 +7909,11 @@
       <c r="I180">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J180" t="s">
-        <v>22</v>
-      </c>
-      <c r="K180" t="s">
-        <v>22</v>
+      <c r="J180">
+        <v>31285000000</v>
+      </c>
+      <c r="K180">
+        <v>0</v>
       </c>
       <c r="L180">
         <v>31</v>
@@ -7944,11 +7947,11 @@
       <c r="I181">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J181" t="s">
-        <v>22</v>
-      </c>
-      <c r="K181" t="s">
-        <v>22</v>
+      <c r="J181">
+        <v>31285000000</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
       </c>
       <c r="L181">
         <v>31</v>
@@ -7982,11 +7985,11 @@
       <c r="I182">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J182" t="s">
-        <v>22</v>
-      </c>
-      <c r="K182" t="s">
-        <v>22</v>
+      <c r="J182">
+        <v>31285000000</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
       </c>
       <c r="L182">
         <v>31</v>
@@ -8020,11 +8023,11 @@
       <c r="I183">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J183" t="s">
-        <v>22</v>
-      </c>
-      <c r="K183" t="s">
-        <v>22</v>
+      <c r="J183">
+        <v>31285000000</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
       </c>
       <c r="L183">
         <v>31</v>
@@ -8058,11 +8061,11 @@
       <c r="I184">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J184" t="s">
-        <v>22</v>
-      </c>
-      <c r="K184" t="s">
-        <v>22</v>
+      <c r="J184">
+        <v>31285000000</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
       </c>
       <c r="L184">
         <v>31</v>
@@ -8096,11 +8099,11 @@
       <c r="I185">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J185" t="s">
-        <v>22</v>
-      </c>
-      <c r="K185" t="s">
-        <v>22</v>
+      <c r="J185">
+        <v>31285000000</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
       </c>
       <c r="L185">
         <v>31</v>
@@ -8134,11 +8137,11 @@
       <c r="I186">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J186" t="s">
-        <v>22</v>
-      </c>
-      <c r="K186" t="s">
-        <v>22</v>
+      <c r="J186">
+        <v>31285000000</v>
+      </c>
+      <c r="K186">
+        <v>0</v>
       </c>
       <c r="L186">
         <v>31</v>
@@ -8172,11 +8175,11 @@
       <c r="I187">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J187" t="s">
-        <v>22</v>
-      </c>
-      <c r="K187" t="s">
-        <v>22</v>
+      <c r="J187">
+        <v>31285000000</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
       </c>
       <c r="L187">
         <v>31</v>
@@ -8210,11 +8213,11 @@
       <c r="I188">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J188" t="s">
-        <v>22</v>
-      </c>
-      <c r="K188" t="s">
-        <v>22</v>
+      <c r="J188">
+        <v>31285000000</v>
+      </c>
+      <c r="K188">
+        <v>0</v>
       </c>
       <c r="L188">
         <v>31</v>
@@ -8248,11 +8251,11 @@
       <c r="I189">
         <v>1.5247031227092801E-2</v>
       </c>
-      <c r="J189" t="s">
-        <v>22</v>
-      </c>
-      <c r="K189" t="s">
-        <v>22</v>
+      <c r="J189">
+        <v>31285000000</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
       </c>
       <c r="L189">
         <v>31</v>
@@ -8289,8 +8292,8 @@
       <c r="J190">
         <v>31285000000</v>
       </c>
-      <c r="K190" t="s">
-        <v>22</v>
+      <c r="K190">
+        <v>0</v>
       </c>
       <c r="L190">
         <v>26</v>
@@ -8327,8 +8330,8 @@
       <c r="J191">
         <v>31285000000</v>
       </c>
-      <c r="K191" t="s">
-        <v>22</v>
+      <c r="K191">
+        <v>0</v>
       </c>
       <c r="L191">
         <v>26</v>
@@ -8365,8 +8368,8 @@
       <c r="J192">
         <v>31285000000</v>
       </c>
-      <c r="K192" t="s">
-        <v>22</v>
+      <c r="K192">
+        <v>0</v>
       </c>
       <c r="L192">
         <v>26</v>
@@ -8403,8 +8406,8 @@
       <c r="J193">
         <v>31285000000</v>
       </c>
-      <c r="K193" t="s">
-        <v>22</v>
+      <c r="K193">
+        <v>0</v>
       </c>
       <c r="L193">
         <v>26</v>
@@ -8441,8 +8444,8 @@
       <c r="J194">
         <v>31285000000</v>
       </c>
-      <c r="K194" t="s">
-        <v>22</v>
+      <c r="K194">
+        <v>0</v>
       </c>
       <c r="L194">
         <v>26</v>
@@ -8479,8 +8482,8 @@
       <c r="J195">
         <v>31285000000</v>
       </c>
-      <c r="K195" t="s">
-        <v>22</v>
+      <c r="K195">
+        <v>0</v>
       </c>
       <c r="L195">
         <v>26</v>
@@ -8517,8 +8520,8 @@
       <c r="J196">
         <v>31285000000</v>
       </c>
-      <c r="K196" t="s">
-        <v>22</v>
+      <c r="K196">
+        <v>0</v>
       </c>
       <c r="L196">
         <v>26</v>
@@ -8555,8 +8558,8 @@
       <c r="J197">
         <v>31285000000</v>
       </c>
-      <c r="K197" t="s">
-        <v>22</v>
+      <c r="K197">
+        <v>0</v>
       </c>
       <c r="L197">
         <v>26</v>
@@ -8593,8 +8596,8 @@
       <c r="J198">
         <v>31285000000</v>
       </c>
-      <c r="K198" t="s">
-        <v>22</v>
+      <c r="K198">
+        <v>0</v>
       </c>
       <c r="L198">
         <v>26</v>
@@ -8631,8 +8634,8 @@
       <c r="J199">
         <v>31285000000</v>
       </c>
-      <c r="K199" t="s">
-        <v>22</v>
+      <c r="K199">
+        <v>0</v>
       </c>
       <c r="L199">
         <v>26</v>
@@ -8669,8 +8672,8 @@
       <c r="J200">
         <v>31285000000</v>
       </c>
-      <c r="K200" t="s">
-        <v>22</v>
+      <c r="K200">
+        <v>0</v>
       </c>
       <c r="L200">
         <v>26</v>
@@ -8707,8 +8710,8 @@
       <c r="J201">
         <v>31285000000</v>
       </c>
-      <c r="K201" t="s">
-        <v>22</v>
+      <c r="K201">
+        <v>0</v>
       </c>
       <c r="L201">
         <v>26</v>
@@ -8745,8 +8748,8 @@
       <c r="J202">
         <v>31285000000</v>
       </c>
-      <c r="K202" t="s">
-        <v>22</v>
+      <c r="K202">
+        <v>0</v>
       </c>
       <c r="L202">
         <v>26</v>
@@ -8783,8 +8786,8 @@
       <c r="J203">
         <v>31285000000</v>
       </c>
-      <c r="K203" t="s">
-        <v>22</v>
+      <c r="K203">
+        <v>0</v>
       </c>
       <c r="L203">
         <v>26</v>
@@ -8821,8 +8824,8 @@
       <c r="J204">
         <v>31285000000</v>
       </c>
-      <c r="K204" t="s">
-        <v>22</v>
+      <c r="K204">
+        <v>0</v>
       </c>
       <c r="L204">
         <v>26</v>
@@ -8859,8 +8862,8 @@
       <c r="J205">
         <v>31285000000</v>
       </c>
-      <c r="K205" t="s">
-        <v>22</v>
+      <c r="K205">
+        <v>0</v>
       </c>
       <c r="L205">
         <v>26</v>

</xml_diff>